<commit_message>
front and backend connect
</commit_message>
<xml_diff>
--- a/server_test/out.xlsx
+++ b/server_test/out.xlsx
@@ -1728,7 +1728,7 @@
       <c r="E4" s="7" t="n"/>
       <c r="F4" s="7" t="n"/>
       <c r="G4" s="10" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H4" s="10" t="n">
         <v>16</v>
@@ -1823,7 +1823,7 @@
         </is>
       </c>
       <c r="G5" s="10" t="n">
-        <v>21.5</v>
+        <v>19.5</v>
       </c>
       <c r="H5" s="10" t="n">
         <v>16</v>
@@ -1916,7 +1916,7 @@
       <c r="E6" s="7" t="n"/>
       <c r="F6" s="7" t="n"/>
       <c r="G6" s="10" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H6" s="10" t="n">
         <v>18</v>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="F7" s="7" t="n"/>
       <c r="G7" s="10" t="n">
-        <v>20.5</v>
+        <v>18.5</v>
       </c>
       <c r="H7" s="10" t="n">
         <v>18</v>
@@ -2108,7 +2108,7 @@
         <v>22</v>
       </c>
       <c r="G8" s="10" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H8" s="10" t="n">
         <v>18</v>
@@ -2205,7 +2205,7 @@
       <c r="E9" s="7" t="n"/>
       <c r="F9" s="7" t="n"/>
       <c r="G9" s="10" t="n">
-        <v>21.5</v>
+        <v>19.5</v>
       </c>
       <c r="H9" s="10" t="n">
         <v>18</v>
@@ -2302,7 +2302,7 @@
       <c r="E10" s="7" t="n"/>
       <c r="F10" s="7" t="n"/>
       <c r="G10" s="10" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H10" s="10" t="n">
         <v>18</v>
@@ -2401,7 +2401,7 @@
         </is>
       </c>
       <c r="G11" s="10" t="n">
-        <v>20.5</v>
+        <v>18.5</v>
       </c>
       <c r="H11" s="10" t="n">
         <v>18</v>
@@ -2494,7 +2494,7 @@
       <c r="E12" s="7" t="n"/>
       <c r="F12" s="7" t="n"/>
       <c r="G12" s="10" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H12" s="10" t="n">
         <v>18</v>
@@ -2593,7 +2593,7 @@
       </c>
       <c r="F13" s="7" t="n"/>
       <c r="G13" s="10" t="n">
-        <v>19.5</v>
+        <v>18</v>
       </c>
       <c r="H13" s="10" t="n">
         <v>18</v>
@@ -2686,7 +2686,7 @@
       <c r="E14" s="7" t="n"/>
       <c r="F14" s="7" t="n"/>
       <c r="G14" s="10" t="n">
-        <v>20</v>
+        <v>18.5</v>
       </c>
       <c r="H14" s="10" t="n">
         <v>22</v>
@@ -2781,7 +2781,7 @@
       <c r="E15" s="7" t="n"/>
       <c r="F15" s="7" t="n"/>
       <c r="G15" s="10" t="n">
-        <v>20.5</v>
+        <v>19</v>
       </c>
       <c r="H15" s="10" t="n">
         <v>22</v>
@@ -2878,7 +2878,7 @@
         </is>
       </c>
       <c r="G16" s="10" t="n">
-        <v>21</v>
+        <v>19.5</v>
       </c>
       <c r="H16" s="10" t="n">
         <v>22</v>
@@ -2971,7 +2971,7 @@
       <c r="E17" s="7" t="n"/>
       <c r="F17" s="7" t="n"/>
       <c r="G17" s="11" t="n">
-        <v>21.5</v>
+        <v>20</v>
       </c>
       <c r="H17" s="11" t="n">
         <v>22</v>
@@ -3072,7 +3072,7 @@
       <c r="E18" s="7" t="n"/>
       <c r="F18" s="7" t="n"/>
       <c r="G18" s="11" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H18" s="10" t="n">
         <v>22</v>
@@ -3096,7 +3096,7 @@
         <v>126.999</v>
       </c>
       <c r="O18" s="19" t="n">
-        <v>23.5</v>
+        <v>24</v>
       </c>
       <c r="P18" s="19" t="n">
         <v>16</v>
@@ -3167,7 +3167,7 @@
         </is>
       </c>
       <c r="G19" s="11" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H19" s="10" t="n">
         <v>22</v>
@@ -3262,7 +3262,7 @@
       <c r="E20" s="7" t="n"/>
       <c r="F20" s="7" t="n"/>
       <c r="G20" s="11" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H20" s="10" t="n">
         <v>22</v>
@@ -3355,7 +3355,7 @@
       <c r="E21" s="7" t="n"/>
       <c r="F21" s="7" t="n"/>
       <c r="G21" s="11" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H21" s="10" t="n">
         <v>22</v>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="F22" s="7" t="n"/>
       <c r="G22" s="11" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H22" s="10" t="n">
         <v>22</v>
@@ -3547,7 +3547,7 @@
       <c r="E23" s="7" t="n"/>
       <c r="F23" s="7" t="n"/>
       <c r="G23" s="11" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H23" s="10" t="n">
         <v>16</v>
@@ -3642,7 +3642,7 @@
         <v>25</v>
       </c>
       <c r="G24" s="11" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H24" s="10" t="n">
         <v>16</v>
@@ -3735,7 +3735,7 @@
       <c r="E25" s="7" t="n"/>
       <c r="F25" s="7" t="n"/>
       <c r="G25" s="10" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H25" s="10" t="n">
         <v>16</v>
@@ -3832,7 +3832,7 @@
       <c r="E26" s="7" t="n"/>
       <c r="F26" s="7" t="n"/>
       <c r="G26" s="10" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H26" s="10" t="n">
         <v>16</v>
@@ -3927,7 +3927,7 @@
         </is>
       </c>
       <c r="G27" s="11" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H27" s="11" t="n">
         <v>16</v>
@@ -4020,7 +4020,7 @@
       <c r="E28" s="7" t="n"/>
       <c r="F28" s="7" t="n"/>
       <c r="G28" s="11" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H28" s="10" t="n">
         <v>16</v>
@@ -4115,7 +4115,7 @@
       </c>
       <c r="F29" s="7" t="n"/>
       <c r="G29" s="10" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H29" s="10" t="n">
         <v>16</v>
@@ -4194,11 +4194,31 @@
           <t>费用小计</t>
         </is>
       </c>
-      <c r="B30" s="7" t="n"/>
-      <c r="C30" s="7" t="n"/>
-      <c r="D30" s="7" t="n"/>
-      <c r="E30" s="7" t="n"/>
-      <c r="F30" s="7" t="n"/>
+      <c r="B30" s="7" t="inlineStr">
+        <is>
+          <t>209.667</t>
+        </is>
+      </c>
+      <c r="C30" s="7" t="inlineStr">
+        <is>
+          <t>376.999</t>
+        </is>
+      </c>
+      <c r="D30" s="7" t="inlineStr">
+        <is>
+          <t>155.667</t>
+        </is>
+      </c>
+      <c r="E30" s="7" t="inlineStr">
+        <is>
+          <t>212.667</t>
+        </is>
+      </c>
+      <c r="F30" s="7" t="inlineStr">
+        <is>
+          <t>113.0</t>
+        </is>
+      </c>
       <c r="G30" s="10" t="n"/>
       <c r="H30" s="10" t="n"/>
       <c r="I30" s="10" t="n"/>
@@ -4368,7 +4388,7 @@
       </c>
       <c r="E34" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:10</t>
+          <t>2024-11-30 21:20:50</t>
         </is>
       </c>
       <c r="F34" s="0" t="inlineStr">
@@ -4384,7 +4404,7 @@
       </c>
       <c r="I34" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:11</t>
+          <t>2024-11-30 21:20:51</t>
         </is>
       </c>
       <c r="J34" s="0" t="inlineStr">
@@ -4400,7 +4420,7 @@
       </c>
       <c r="M34" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:12</t>
+          <t>2024-11-30 21:20:52</t>
         </is>
       </c>
       <c r="N34" s="0" t="inlineStr">
@@ -4416,7 +4436,7 @@
       </c>
       <c r="Q34" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:13</t>
+          <t>2024-11-30 21:20:53</t>
         </is>
       </c>
       <c r="R34" s="0" t="inlineStr">
@@ -4432,7 +4452,7 @@
       </c>
       <c r="U34" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:11</t>
+          <t>2024-11-30 21:20:51</t>
         </is>
       </c>
     </row>
@@ -4450,7 +4470,7 @@
       </c>
       <c r="E35" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:11</t>
+          <t>2024-11-30 21:20:51</t>
         </is>
       </c>
       <c r="F35" s="0" t="inlineStr">
@@ -4466,7 +4486,7 @@
       </c>
       <c r="I35" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:13</t>
+          <t>2024-11-30 21:20:53</t>
         </is>
       </c>
       <c r="J35" s="0" t="inlineStr">
@@ -4482,7 +4502,7 @@
       </c>
       <c r="M35" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:13</t>
+          <t>2024-11-30 21:20:53</t>
         </is>
       </c>
       <c r="N35" s="0" t="inlineStr">
@@ -4498,7 +4518,7 @@
       </c>
       <c r="Q35" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:14</t>
+          <t>2024-11-30 21:20:54</t>
         </is>
       </c>
       <c r="R35" s="0" t="inlineStr">
@@ -4514,7 +4534,7 @@
       </c>
       <c r="U35" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:14</t>
+          <t>2024-11-30 21:20:54</t>
         </is>
       </c>
     </row>
@@ -4532,7 +4552,7 @@
       </c>
       <c r="E36" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:13</t>
+          <t>2024-11-30 21:20:53</t>
         </is>
       </c>
       <c r="F36" s="0" t="inlineStr">
@@ -4548,7 +4568,7 @@
       </c>
       <c r="I36" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:14</t>
+          <t>2024-11-30 21:20:54</t>
         </is>
       </c>
       <c r="J36" s="0" t="inlineStr">
@@ -4564,7 +4584,7 @@
       </c>
       <c r="M36" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:16</t>
+          <t>2024-11-30 21:20:56</t>
         </is>
       </c>
       <c r="N36" s="0" t="inlineStr">
@@ -4580,7 +4600,7 @@
       </c>
       <c r="Q36" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:18</t>
+          <t>2024-11-30 21:20:58</t>
         </is>
       </c>
       <c r="R36" s="0" t="inlineStr">
@@ -4596,7 +4616,7 @@
       </c>
       <c r="U36" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:15</t>
+          <t>2024-11-30 21:20:55</t>
         </is>
       </c>
     </row>
@@ -4614,7 +4634,7 @@
       </c>
       <c r="E37" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:15</t>
+          <t>2024-11-30 21:20:55</t>
         </is>
       </c>
       <c r="F37" s="0" t="inlineStr">
@@ -4630,7 +4650,7 @@
       </c>
       <c r="I37" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:16</t>
+          <t>2024-11-30 21:20:56</t>
         </is>
       </c>
       <c r="J37" s="0" t="inlineStr">
@@ -4646,7 +4666,7 @@
       </c>
       <c r="M37" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:18</t>
+          <t>2024-11-30 21:20:58</t>
         </is>
       </c>
       <c r="N37" s="0" t="inlineStr">
@@ -4662,7 +4682,7 @@
       </c>
       <c r="Q37" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:19</t>
+          <t>2024-11-30 21:20:59</t>
         </is>
       </c>
       <c r="R37" s="0" t="inlineStr">
@@ -4678,7 +4698,7 @@
       </c>
       <c r="U37" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:16</t>
+          <t>2024-11-30 21:20:56</t>
         </is>
       </c>
     </row>
@@ -4696,7 +4716,7 @@
       </c>
       <c r="E38" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:15</t>
+          <t>2024-11-30 21:20:55</t>
         </is>
       </c>
       <c r="F38" s="0" t="inlineStr">
@@ -4712,7 +4732,7 @@
       </c>
       <c r="I38" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:17</t>
+          <t>2024-11-30 21:20:57</t>
         </is>
       </c>
       <c r="J38" s="0" t="inlineStr">
@@ -4728,7 +4748,7 @@
       </c>
       <c r="M38" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:18</t>
+          <t>2024-11-30 21:20:58</t>
         </is>
       </c>
       <c r="N38" s="0" t="inlineStr">
@@ -4744,7 +4764,7 @@
       </c>
       <c r="Q38" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:19</t>
+          <t>2024-11-30 21:20:59</t>
         </is>
       </c>
       <c r="R38" s="0" t="inlineStr">
@@ -4760,7 +4780,7 @@
       </c>
       <c r="U38" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:17</t>
+          <t>2024-11-30 21:20:57</t>
         </is>
       </c>
     </row>
@@ -4778,7 +4798,7 @@
       </c>
       <c r="E39" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:19</t>
+          <t>2024-11-30 21:20:59</t>
         </is>
       </c>
       <c r="F39" s="0" t="inlineStr">
@@ -4794,7 +4814,7 @@
       </c>
       <c r="I39" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:18</t>
+          <t>2024-11-30 21:20:58</t>
         </is>
       </c>
       <c r="J39" s="0" t="inlineStr">
@@ -4810,7 +4830,7 @@
       </c>
       <c r="M39" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:22</t>
+          <t>2024-11-30 21:21:02</t>
         </is>
       </c>
       <c r="N39" s="0" t="inlineStr">
@@ -4826,7 +4846,7 @@
       </c>
       <c r="Q39" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:19</t>
+          <t>2024-11-30 21:20:59</t>
         </is>
       </c>
       <c r="R39" s="0" t="inlineStr">
@@ -4842,7 +4862,7 @@
       </c>
       <c r="U39" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:22</t>
+          <t>2024-11-30 21:21:02</t>
         </is>
       </c>
     </row>
@@ -4860,7 +4880,7 @@
       </c>
       <c r="E40" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:24</t>
+          <t>2024-11-30 21:21:04</t>
         </is>
       </c>
       <c r="F40" s="0" t="inlineStr">
@@ -4876,7 +4896,7 @@
       </c>
       <c r="I40" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:19</t>
+          <t>2024-11-30 21:20:59</t>
         </is>
       </c>
       <c r="J40" s="0" t="inlineStr">
@@ -4892,7 +4912,7 @@
       </c>
       <c r="M40" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:22</t>
+          <t>2024-11-30 21:21:02</t>
         </is>
       </c>
       <c r="N40" s="0" t="inlineStr">
@@ -4908,7 +4928,7 @@
       </c>
       <c r="Q40" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:27</t>
+          <t>2024-11-30 21:21:07</t>
         </is>
       </c>
       <c r="R40" s="0" t="inlineStr">
@@ -4924,7 +4944,7 @@
       </c>
       <c r="U40" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:22</t>
+          <t>2024-11-30 21:21:02</t>
         </is>
       </c>
     </row>
@@ -4942,7 +4962,7 @@
       </c>
       <c r="E41" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:28</t>
+          <t>2024-11-30 21:21:08</t>
         </is>
       </c>
       <c r="F41" s="0" t="inlineStr">
@@ -4958,7 +4978,7 @@
       </c>
       <c r="I41" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:21</t>
+          <t>2024-11-30 21:21:01</t>
         </is>
       </c>
       <c r="J41" s="0" t="inlineStr">
@@ -4974,7 +4994,7 @@
       </c>
       <c r="M41" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:23</t>
+          <t>2024-11-30 21:21:03</t>
         </is>
       </c>
       <c r="N41" s="0" t="inlineStr">
@@ -4990,7 +5010,7 @@
       </c>
       <c r="Q41" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:28</t>
+          <t>2024-11-30 21:21:08</t>
         </is>
       </c>
       <c r="R41" s="0" t="inlineStr">
@@ -5006,7 +5026,7 @@
       </c>
       <c r="U41" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:23</t>
+          <t>2024-11-30 21:21:03</t>
         </is>
       </c>
     </row>
@@ -5024,7 +5044,7 @@
       </c>
       <c r="E42" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:28</t>
+          <t>2024-11-30 21:21:08</t>
         </is>
       </c>
       <c r="F42" s="0" t="inlineStr">
@@ -5040,7 +5060,7 @@
       </c>
       <c r="I42" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:22</t>
+          <t>2024-11-30 21:21:02</t>
         </is>
       </c>
       <c r="J42" s="0" t="inlineStr">
@@ -5056,7 +5076,7 @@
       </c>
       <c r="M42" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:24</t>
+          <t>2024-11-30 21:21:04</t>
         </is>
       </c>
       <c r="N42" s="0" t="inlineStr">
@@ -5072,7 +5092,7 @@
       </c>
       <c r="Q42" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:28</t>
+          <t>2024-11-30 21:21:08</t>
         </is>
       </c>
       <c r="R42" s="0" t="inlineStr">
@@ -5088,7 +5108,7 @@
       </c>
       <c r="U42" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:23</t>
+          <t>2024-11-30 21:21:03</t>
         </is>
       </c>
     </row>
@@ -5106,7 +5126,7 @@
       </c>
       <c r="E43" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:34</t>
+          <t>2024-11-30 21:21:14</t>
         </is>
       </c>
       <c r="F43" s="0" t="inlineStr">
@@ -5122,7 +5142,7 @@
       </c>
       <c r="I43" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:23</t>
+          <t>2024-11-30 21:21:03</t>
         </is>
       </c>
       <c r="J43" s="0" t="inlineStr">
@@ -5138,7 +5158,7 @@
       </c>
       <c r="M43" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:24</t>
+          <t>2024-11-30 21:21:04</t>
         </is>
       </c>
       <c r="N43" s="0" t="inlineStr">
@@ -5154,7 +5174,7 @@
       </c>
       <c r="Q43" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:28</t>
+          <t>2024-11-30 21:21:08</t>
         </is>
       </c>
       <c r="R43" s="0" t="inlineStr">
@@ -5170,57 +5190,57 @@
       </c>
       <c r="U43" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:50:25</t>
+          <t>2024-11-30 21:21:05</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="B44" s="0" t="inlineStr">
         <is>
-          <t>removed from serve queue</t>
+          <t>turn off</t>
         </is>
       </c>
       <c r="C44" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>107.333</v>
+        <v>109</v>
       </c>
       <c r="E44" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:49:26</t>
+          <t>2024-11-30 21:11:19</t>
         </is>
       </c>
       <c r="F44" s="0" t="inlineStr">
         <is>
+          <t>turn off</t>
+        </is>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>125.999</v>
+      </c>
+      <c r="I44" s="0" t="inlineStr">
+        <is>
+          <t>2024-11-30 21:11:11</t>
+        </is>
+      </c>
+      <c r="J44" s="0" t="inlineStr">
+        <is>
           <t>add to serve queue</t>
-        </is>
-      </c>
-      <c r="G44" s="0" t="n">
-        <v>0.33333</v>
-      </c>
-      <c r="H44" s="0" t="n">
-        <v>251</v>
-      </c>
-      <c r="I44" s="0" t="inlineStr">
-        <is>
-          <t>2024-11-29 22:49:32</t>
-        </is>
-      </c>
-      <c r="J44" s="0" t="inlineStr">
-        <is>
-          <t>removed from serve queue</t>
         </is>
       </c>
       <c r="K44" s="0" t="n">
         <v>0.33333</v>
       </c>
       <c r="L44" s="0" t="n">
-        <v>2.33331</v>
+        <v>0.99999</v>
       </c>
       <c r="M44" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:45:07</t>
+          <t>2024-11-30 21:11:12</t>
         </is>
       </c>
       <c r="N44" s="0" t="inlineStr">
@@ -5241,18 +5261,18 @@
       </c>
       <c r="R44" s="0" t="inlineStr">
         <is>
-          <t>add to serve queue</t>
+          <t>turn off</t>
         </is>
       </c>
       <c r="S44" s="0" t="n">
-        <v>0.33333</v>
+        <v>1</v>
       </c>
       <c r="T44" s="0" t="n">
-        <v>3.99999</v>
+        <v>18.6666</v>
       </c>
       <c r="U44" s="0" t="inlineStr">
         <is>
-          <t>2024-11-29 22:49:23</t>
+          <t>2024-11-30 21:11:18</t>
         </is>
       </c>
     </row>

</xml_diff>